<commit_message>
ADX-485 Regenerate data templates.
</commit_message>
<xml_diff>
--- a/excel_templates/Inputs to UNAIDS Estimates 2020/art_inputs.xlsx
+++ b/excel_templates/Inputs to UNAIDS Estimates 2020/art_inputs.xlsx
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t xml:space="preserve">UNAIDS ART Programme Input | Data Template</t>
   </si>
   <si>
-    <t xml:space="preserve">version 2.0; 2020-08-14</t>
+    <t xml:space="preserve">version 2.1; 2020-11-10</t>
   </si>
   <si>
     <t xml:space="preserve">Please use the following definitions to fill in the template overleaf. If data does not exist, please indicate so with the value "NA" and ignore any warning given by Excel.</t>
@@ -92,16 +92,10 @@
     <t xml:space="preserve">case sensitive restricted values: "Y000_014", "Y015_999", "Y000_999"</t>
   </si>
   <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The year.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minimum: 1970|maximum: 2021</t>
+    <t xml:space="preserve">calendar_quarter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The calendar quarter reflected the end of reporting period. Formatted as CY20XXQY, for example CY2020Q4 for end of December 2020.</t>
   </si>
   <si>
     <t xml:space="preserve">art_current</t>
@@ -114,12 +108,6 @@
   </si>
   <si>
     <t xml:space="preserve">minimum: 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">art_new</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number newly initiating ART during the reporting period (year).</t>
   </si>
   <si>
     <t xml:space="preserve">** For each row, the fields that contribute to the unique key must form a unique combination of values across the data set.</t>
@@ -261,12 +249,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -332,26 +320,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="79.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="113.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="60.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.8"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -361,7 +350,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -371,7 +360,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -381,7 +370,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -401,7 +390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>9</v>
       </c>
@@ -421,7 +410,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>14</v>
       </c>
@@ -438,7 +427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>17</v>
       </c>
@@ -458,7 +447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>20</v>
       </c>
@@ -478,7 +467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>23</v>
       </c>
@@ -486,76 +475,59 @@
         <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A19:F19"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -568,25 +540,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,13 +577,24 @@
         <v>23</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C1001" type="list">
+      <formula1>"both,male,female"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D1001" type="list">
+      <formula1>"Y000_014,Y015_999,Y000_999"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F2:F1001" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>